<commit_message>
Update documentation and design description
</commit_message>
<xml_diff>
--- a/Documentation/Spinning LED Design Calculations.xlsx
+++ b/Documentation/Spinning LED Design Calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joris\Development\SpinningLED\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B641DF6-F05E-4C61-BEFA-0DCDBB0D42D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDD7DBB-1EC1-4F94-9161-3811D3540F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8730" yWindow="1005" windowWidth="29775" windowHeight="19695" activeTab="2" xr2:uid="{E62B6D04-78E4-41CC-9A69-00D259FBE61F}"/>
+    <workbookView xWindow="10125" yWindow="2925" windowWidth="27660" windowHeight="17610" activeTab="1" xr2:uid="{E62B6D04-78E4-41CC-9A69-00D259FBE61F}"/>
   </bookViews>
   <sheets>
     <sheet name="Centrifugal Force &amp; Speed" sheetId="1" r:id="rId1"/>
@@ -39,8 +39,37 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Joris</author>
+  </authors>
+  <commentList>
+    <comment ref="F42" authorId="0" shapeId="0" xr:uid="{21D520EE-9596-4E91-BB1B-86EF5F0E709E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Per STM32 application note:
+Accuracy of Factory Calibrated HSI16 oscillator:
+-1.5% to 1.5%    VDDA =3.0V 0-55 degC
+-2% to 2%          VDDA =3.0V -10-70 degC
+-2.5% to 2%       VDDA =3.0V -10-85 degC
+We should be within 2%.
+dm00425536-how-to-optimize-stm32-mcus-internal-rc-oscillator-accuracy-stmicroelectronics-1.pdf</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="61">
   <si>
     <t>Inputs</t>
   </si>
@@ -198,9 +227,6 @@
     <t xml:space="preserve"> 144 LED strip spacing</t>
   </si>
   <si>
-    <t>144 LED strip interlaced spacing</t>
-  </si>
-  <si>
     <t>Pixels around</t>
   </si>
   <si>
@@ -220,12 +246,6 @@
   </si>
   <si>
     <t>Memory (KB) - RGB565 + buffer</t>
-  </si>
-  <si>
-    <t>SPI Freq (MHz)</t>
-  </si>
-  <si>
-    <t>MHz</t>
   </si>
   <si>
     <t>Accuracy</t>
@@ -304,6 +324,21 @@
   <si>
     <t>/</t>
   </si>
+  <si>
+    <t>SPI Freq (Mbps)</t>
+  </si>
+  <si>
+    <t>Mbps</t>
+  </si>
+  <si>
+    <t>INTERLACED - 144 LED strip spacing</t>
+  </si>
+  <si>
+    <t>SPI Frequency</t>
+  </si>
+  <si>
+    <t>LEDs high</t>
+  </si>
 </sst>
 </file>
 
@@ -313,7 +348,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,8 +411,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -394,6 +442,11 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -424,11 +477,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -461,7 +515,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -469,16 +522,203 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="39">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3108,11 +3348,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A950B1B-D92C-4C21-8227-ACDCFF31358D}">
-  <dimension ref="A4:AK51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A950B1B-D92C-4C21-8227-ACDCFF31358D}">
+  <dimension ref="A4:AK52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3130,40 +3370,40 @@
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="32"/>
-      <c r="G6" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
+      <c r="B6" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="33"/>
+      <c r="G6" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
-      <c r="X6" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y6" s="32"/>
-      <c r="Z6" s="32"/>
-      <c r="AA6" s="32"/>
-      <c r="AB6" s="32"/>
-      <c r="AC6" s="32"/>
-      <c r="AD6" s="32"/>
-      <c r="AE6" s="32"/>
+      <c r="X6" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y6" s="33"/>
+      <c r="Z6" s="33"/>
+      <c r="AA6" s="33"/>
+      <c r="AB6" s="33"/>
+      <c r="AC6" s="33"/>
+      <c r="AD6" s="33"/>
+      <c r="AE6" s="33"/>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>288</v>
@@ -3247,7 +3487,7 @@
       <c r="AG7" s="5">
         <v>144</v>
       </c>
-      <c r="AH7" s="13">
+      <c r="AH7" s="34">
         <v>288</v>
       </c>
       <c r="AI7" s="14">
@@ -3368,7 +3608,7 @@
         <f t="shared" si="3"/>
         <v>6.9444444444444446</v>
       </c>
-      <c r="AH8" s="15">
+      <c r="AH8" s="35">
         <f t="shared" si="3"/>
         <v>3.4722222222222223</v>
       </c>
@@ -3389,7 +3629,7 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="F9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" s="5">
         <v>2</v>
@@ -3434,7 +3674,7 @@
         <v>1</v>
       </c>
       <c r="W9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X9" s="5">
         <v>2</v>
@@ -3466,7 +3706,7 @@
       <c r="AG9" s="5">
         <v>1</v>
       </c>
-      <c r="AH9" s="13">
+      <c r="AH9" s="34">
         <v>2</v>
       </c>
       <c r="AI9" s="14">
@@ -3483,7 +3723,7 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="F10" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" s="5">
         <v>0.15</v>
@@ -3528,7 +3768,7 @@
         <v>0.5</v>
       </c>
       <c r="W10" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X10" s="5">
         <v>0.15</v>
@@ -3560,7 +3800,7 @@
       <c r="AG10" s="5">
         <v>0.35</v>
       </c>
-      <c r="AH10" s="13">
+      <c r="AH10" s="34">
         <v>0.4</v>
       </c>
       <c r="AI10" s="14">
@@ -3578,7 +3818,7 @@
         <v>20</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" s="5">
         <f>ROUND(G10*G7/G9,0)*G9</f>
@@ -3637,7 +3877,7 @@
         <v>72</v>
       </c>
       <c r="W11" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="X11" s="5">
         <f t="shared" ref="X11:AI11" si="8">ROUND(X10*X7/X9,0)*X9</f>
@@ -3679,7 +3919,7 @@
         <f t="shared" si="8"/>
         <v>50</v>
       </c>
-      <c r="AH11" s="13">
+      <c r="AH11" s="34">
         <f t="shared" si="8"/>
         <v>116</v>
       </c>
@@ -3952,127 +4192,127 @@
         <v>26.1181640625</v>
       </c>
     </row>
-    <row r="14" spans="1:37" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26">
+    <row r="14" spans="1:37" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="25">
         <v>0.22</v>
       </c>
-      <c r="B14" s="27">
+      <c r="B14" s="26">
         <f t="shared" si="17"/>
         <v>398.10262106289855</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="26">
         <f t="shared" si="17"/>
         <v>199.05131053144927</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="26">
         <f t="shared" si="11"/>
         <v>68.921875</v>
       </c>
-      <c r="H14" s="27">
+      <c r="H14" s="26">
         <f t="shared" si="11"/>
         <v>17.359375</v>
       </c>
-      <c r="I14" s="29">
+      <c r="I14" s="28">
         <f t="shared" si="11"/>
         <v>90.8515625</v>
       </c>
-      <c r="J14" s="30">
+      <c r="J14" s="29">
         <f t="shared" si="11"/>
         <v>22.8828125</v>
       </c>
-      <c r="K14" s="27">
+      <c r="K14" s="26">
         <f t="shared" si="11"/>
         <v>112.78125</v>
       </c>
-      <c r="L14" s="27">
+      <c r="L14" s="26">
         <f t="shared" si="11"/>
         <v>28.40625</v>
       </c>
-      <c r="M14" s="29">
+      <c r="M14" s="28">
         <f t="shared" si="11"/>
         <v>134.7109375</v>
       </c>
-      <c r="N14" s="30">
+      <c r="N14" s="29">
         <f t="shared" si="11"/>
         <v>33.9296875</v>
       </c>
-      <c r="O14" s="27">
+      <c r="O14" s="26">
         <f t="shared" si="11"/>
         <v>156.640625</v>
       </c>
-      <c r="P14" s="27">
+      <c r="P14" s="26">
         <f t="shared" si="11"/>
         <v>39.453125</v>
       </c>
-      <c r="Q14" s="29">
+      <c r="Q14" s="28">
         <f t="shared" si="11"/>
         <v>181.703125</v>
       </c>
-      <c r="R14" s="30">
+      <c r="R14" s="29">
         <f t="shared" si="11"/>
         <v>45.765625</v>
       </c>
-      <c r="S14" s="29">
+      <c r="S14" s="28">
         <f t="shared" si="11"/>
         <v>225.5625</v>
       </c>
-      <c r="T14" s="30">
+      <c r="T14" s="29">
         <f t="shared" si="11"/>
         <v>56.8125</v>
       </c>
-      <c r="X14" s="27">
+      <c r="X14" s="26">
         <f t="shared" si="18"/>
         <v>34.332249496922351</v>
       </c>
-      <c r="Y14" s="27">
+      <c r="Y14" s="26">
         <f t="shared" si="19"/>
         <v>8.6310059518525097</v>
       </c>
-      <c r="Z14" s="29">
+      <c r="Z14" s="28">
         <f t="shared" si="20"/>
         <v>45.242183224908239</v>
       </c>
-      <c r="AA14" s="30">
+      <c r="AA14" s="29">
         <f t="shared" si="21"/>
         <v>11.365260157091864</v>
       </c>
-      <c r="AB14" s="27">
+      <c r="AB14" s="26">
         <f t="shared" si="22"/>
         <v>56.152205997043183</v>
       </c>
-      <c r="AC14" s="27">
+      <c r="AC14" s="26">
         <f t="shared" si="23"/>
         <v>14.09956275092231</v>
       </c>
-      <c r="AD14" s="29">
+      <c r="AD14" s="28">
         <f t="shared" si="24"/>
         <v>67.062273276868723</v>
       </c>
-      <c r="AE14" s="30">
+      <c r="AE14" s="29">
         <f t="shared" si="25"/>
         <v>16.833889510280404</v>
       </c>
-      <c r="AF14" s="27">
+      <c r="AF14" s="26">
         <f t="shared" si="13"/>
         <v>77.972365984235495</v>
       </c>
-      <c r="AG14" s="27">
+      <c r="AG14" s="26">
         <f t="shared" si="14"/>
         <v>19.56823006766183</v>
       </c>
-      <c r="AH14" s="31">
+      <c r="AH14" s="30">
         <f t="shared" si="15"/>
         <v>90.441068254668139</v>
       </c>
-      <c r="AI14" s="30">
+      <c r="AI14" s="29">
         <f t="shared" si="16"/>
         <v>22.693204090513031</v>
       </c>
-      <c r="AJ14" s="29">
+      <c r="AJ14" s="28">
         <f t="shared" si="15"/>
         <v>112.26131407419841</v>
       </c>
-      <c r="AK14" s="30">
+      <c r="AK14" s="29">
         <f t="shared" si="16"/>
         <v>28.16191800435384</v>
       </c>
@@ -4839,29 +5079,69 @@
         <v>63.75447922092993</v>
       </c>
     </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AH21" s="36"/>
+    </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M24" s="5">
+        <v>58</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="P24" s="32">
+        <f>F42</f>
+        <v>0.02</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>34</v>
+      </c>
+      <c r="R24" s="24">
+        <f>H42</f>
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="S24" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
-      <c r="B25" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32" t="s">
+      <c r="B25" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="L25" s="33" t="str">
+        <f>B25</f>
+        <v>INTERLACED - 144 LED strip spacing</v>
+      </c>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
+      <c r="P25" s="33" t="str">
+        <f>F25</f>
+        <v xml:space="preserve"> 144 LED strip spacing</v>
+      </c>
+      <c r="Q25" s="33"/>
+      <c r="R25" s="33"/>
+      <c r="S25" s="33"/>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="21">
         <v>288</v>
@@ -4887,10 +5167,42 @@
       <c r="I26" s="21">
         <v>144</v>
       </c>
+      <c r="L26" s="5">
+        <f>B26</f>
+        <v>288</v>
+      </c>
+      <c r="M26" s="5">
+        <f>C26</f>
+        <v>288</v>
+      </c>
+      <c r="N26" s="5">
+        <f>D26</f>
+        <v>288</v>
+      </c>
+      <c r="O26" s="5">
+        <f>E26</f>
+        <v>288</v>
+      </c>
+      <c r="P26" s="5">
+        <f>F26</f>
+        <v>144</v>
+      </c>
+      <c r="Q26" s="5">
+        <f>G26</f>
+        <v>144</v>
+      </c>
+      <c r="R26" s="5">
+        <f>H26</f>
+        <v>144</v>
+      </c>
+      <c r="S26" s="5">
+        <f>I26</f>
+        <v>144</v>
+      </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" s="21">
         <v>2</v>
@@ -4914,6 +5226,38 @@
         <v>1</v>
       </c>
       <c r="I27" s="21">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <f>B27</f>
+        <v>2</v>
+      </c>
+      <c r="M27">
+        <f>C27</f>
+        <v>2</v>
+      </c>
+      <c r="N27">
+        <f>D27</f>
+        <v>2</v>
+      </c>
+      <c r="O27">
+        <f>E27</f>
+        <v>2</v>
+      </c>
+      <c r="P27">
+        <f>F27</f>
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <f>G27</f>
+        <v>1</v>
+      </c>
+      <c r="R27">
+        <f>H27</f>
+        <v>1</v>
+      </c>
+      <c r="S27">
+        <f>I27</f>
         <v>1</v>
       </c>
     </row>
@@ -4953,6 +5297,38 @@
         <f t="shared" si="28"/>
         <v>6.9444444444444446</v>
       </c>
+      <c r="L28" s="3">
+        <f>B28</f>
+        <v>3.4722222222222223</v>
+      </c>
+      <c r="M28" s="3">
+        <f>C28</f>
+        <v>3.4722222222222223</v>
+      </c>
+      <c r="N28" s="3">
+        <f>D28</f>
+        <v>3.4722222222222223</v>
+      </c>
+      <c r="O28" s="3">
+        <f>E28</f>
+        <v>3.4722222222222223</v>
+      </c>
+      <c r="P28" s="3">
+        <f>F28</f>
+        <v>6.9444444444444446</v>
+      </c>
+      <c r="Q28" s="3">
+        <f>G28</f>
+        <v>6.9444444444444446</v>
+      </c>
+      <c r="R28" s="3">
+        <f>H28</f>
+        <v>6.9444444444444446</v>
+      </c>
+      <c r="S28" s="3">
+        <f>I28</f>
+        <v>6.9444444444444446</v>
+      </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
@@ -4982,6 +5358,38 @@
       <c r="I29">
         <v>30</v>
       </c>
+      <c r="L29">
+        <f>B29</f>
+        <v>15</v>
+      </c>
+      <c r="M29">
+        <f>C29</f>
+        <v>20</v>
+      </c>
+      <c r="N29">
+        <f>D29</f>
+        <v>25</v>
+      </c>
+      <c r="O29">
+        <f>E29</f>
+        <v>30</v>
+      </c>
+      <c r="P29">
+        <f>F29</f>
+        <v>15</v>
+      </c>
+      <c r="Q29">
+        <f>G29</f>
+        <v>20</v>
+      </c>
+      <c r="R29">
+        <f>H29</f>
+        <v>25</v>
+      </c>
+      <c r="S29">
+        <f>I29</f>
+        <v>30</v>
+      </c>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
@@ -5027,13 +5435,45 @@
         <f t="shared" si="29"/>
         <v>4071.5040790523717</v>
       </c>
+      <c r="L31" s="3">
+        <f>B31*(4*$M$24+8)*8/1000000*(1+$P$24)*(1+$R$24)</f>
+        <v>8.0772908250655746</v>
+      </c>
+      <c r="M31" s="3">
+        <f t="shared" ref="M31:S39" si="30">C31*(4*$M$24+8)*8/1000000*(1+$P$24)*(1+$R$24)</f>
+        <v>10.769721100087432</v>
+      </c>
+      <c r="N31" s="3">
+        <f t="shared" si="30"/>
+        <v>13.46215137510929</v>
+      </c>
+      <c r="O31" s="3">
+        <f t="shared" si="30"/>
+        <v>16.154581650131149</v>
+      </c>
+      <c r="P31" s="3">
+        <f t="shared" si="30"/>
+        <v>4.0386454125327873</v>
+      </c>
+      <c r="Q31" s="3">
+        <f t="shared" si="30"/>
+        <v>5.3848605500437161</v>
+      </c>
+      <c r="R31" s="3">
+        <f t="shared" si="30"/>
+        <v>6.7310756875546449</v>
+      </c>
+      <c r="S31" s="3">
+        <f t="shared" si="30"/>
+        <v>8.0772908250655746</v>
+      </c>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>0.2</v>
       </c>
       <c r="B32" s="12">
-        <f t="shared" ref="B32:B39" si="30">2*PI()*$A32/B$28*1000*B$29</f>
+        <f t="shared" ref="B32:B39" si="31">2*PI()*$A32/B$28*1000*B$29</f>
         <v>5428.6721054031623</v>
       </c>
       <c r="C32" s="12">
@@ -5064,13 +5504,45 @@
         <f t="shared" si="29"/>
         <v>5428.6721054031623</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L32" s="3">
+        <f t="shared" ref="L32:L39" si="32">B32*(4*$M$24+8)*8/1000000*(1+$P$24)*(1+$R$24)</f>
+        <v>10.769721100087432</v>
+      </c>
+      <c r="M32" s="3">
+        <f t="shared" si="30"/>
+        <v>14.35962813344991</v>
+      </c>
+      <c r="N32" s="3">
+        <f t="shared" si="30"/>
+        <v>17.949535166812389</v>
+      </c>
+      <c r="O32" s="3">
+        <f t="shared" si="30"/>
+        <v>21.539442200174864</v>
+      </c>
+      <c r="P32" s="3">
+        <f t="shared" si="30"/>
+        <v>5.3848605500437161</v>
+      </c>
+      <c r="Q32" s="3">
+        <f t="shared" si="30"/>
+        <v>7.1798140667249548</v>
+      </c>
+      <c r="R32" s="3">
+        <f t="shared" si="30"/>
+        <v>8.9747675834061944</v>
+      </c>
+      <c r="S32" s="3">
+        <f t="shared" si="30"/>
+        <v>10.769721100087432</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>0.22</v>
       </c>
       <c r="B33" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>5971.539315943478</v>
       </c>
       <c r="C33" s="12">
@@ -5101,13 +5573,45 @@
         <f t="shared" si="29"/>
         <v>5971.539315943478</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L33" s="3">
+        <f t="shared" si="32"/>
+        <v>11.846693210096175</v>
+      </c>
+      <c r="M33" s="3">
+        <f t="shared" si="30"/>
+        <v>15.795590946794901</v>
+      </c>
+      <c r="N33" s="3">
+        <f t="shared" si="30"/>
+        <v>19.744488683493625</v>
+      </c>
+      <c r="O33" s="3">
+        <f t="shared" si="30"/>
+        <v>23.693386420192351</v>
+      </c>
+      <c r="P33" s="3">
+        <f t="shared" si="30"/>
+        <v>5.9233466050480876</v>
+      </c>
+      <c r="Q33" s="3">
+        <f t="shared" si="30"/>
+        <v>7.8977954733974505</v>
+      </c>
+      <c r="R33" s="3">
+        <f t="shared" si="30"/>
+        <v>9.8722443417468124</v>
+      </c>
+      <c r="S33" s="3">
+        <f t="shared" si="30"/>
+        <v>11.846693210096175</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>0.25</v>
       </c>
       <c r="B34" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>6785.8401317539528</v>
       </c>
       <c r="C34" s="12">
@@ -5138,13 +5642,45 @@
         <f t="shared" si="29"/>
         <v>6785.8401317539528</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L34" s="3">
+        <f t="shared" si="32"/>
+        <v>13.46215137510929</v>
+      </c>
+      <c r="M34" s="3">
+        <f t="shared" si="30"/>
+        <v>17.949535166812389</v>
+      </c>
+      <c r="N34" s="3">
+        <f t="shared" si="30"/>
+        <v>22.436918958515484</v>
+      </c>
+      <c r="O34" s="3">
+        <f t="shared" si="30"/>
+        <v>26.92430275021858</v>
+      </c>
+      <c r="P34" s="3">
+        <f t="shared" si="30"/>
+        <v>6.7310756875546449</v>
+      </c>
+      <c r="Q34" s="3">
+        <f t="shared" si="30"/>
+        <v>8.9747675834061944</v>
+      </c>
+      <c r="R34" s="3">
+        <f t="shared" si="30"/>
+        <v>11.218459479257742</v>
+      </c>
+      <c r="S34" s="3">
+        <f t="shared" si="30"/>
+        <v>13.46215137510929</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>0.3</v>
       </c>
       <c r="B35" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>8143.0081581047434</v>
       </c>
       <c r="C35" s="12">
@@ -5175,13 +5711,45 @@
         <f t="shared" si="29"/>
         <v>8143.0081581047434</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L35" s="3">
+        <f t="shared" si="32"/>
+        <v>16.154581650131149</v>
+      </c>
+      <c r="M35" s="3">
+        <f t="shared" si="30"/>
+        <v>21.539442200174864</v>
+      </c>
+      <c r="N35" s="3">
+        <f t="shared" si="30"/>
+        <v>26.92430275021858</v>
+      </c>
+      <c r="O35" s="3">
+        <f t="shared" si="30"/>
+        <v>32.309163300262298</v>
+      </c>
+      <c r="P35" s="3">
+        <f t="shared" si="30"/>
+        <v>8.0772908250655746</v>
+      </c>
+      <c r="Q35" s="3">
+        <f t="shared" si="30"/>
+        <v>10.769721100087432</v>
+      </c>
+      <c r="R35" s="3">
+        <f t="shared" si="30"/>
+        <v>13.46215137510929</v>
+      </c>
+      <c r="S35" s="3">
+        <f t="shared" si="30"/>
+        <v>16.154581650131149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>0.35</v>
       </c>
       <c r="B36" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>9500.1761844555331</v>
       </c>
       <c r="C36" s="3">
@@ -5212,13 +5780,45 @@
         <f t="shared" si="29"/>
         <v>9500.1761844555331</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L36" s="3">
+        <f t="shared" si="32"/>
+        <v>18.847011925153005</v>
+      </c>
+      <c r="M36" s="3">
+        <f t="shared" si="30"/>
+        <v>25.12934923353734</v>
+      </c>
+      <c r="N36" s="3">
+        <f t="shared" si="30"/>
+        <v>31.411686541921675</v>
+      </c>
+      <c r="O36" s="3">
+        <f t="shared" si="30"/>
+        <v>37.69402385030601</v>
+      </c>
+      <c r="P36" s="3">
+        <f t="shared" si="30"/>
+        <v>9.4235059625765025</v>
+      </c>
+      <c r="Q36" s="3">
+        <f t="shared" si="30"/>
+        <v>12.56467461676867</v>
+      </c>
+      <c r="R36" s="3">
+        <f t="shared" si="30"/>
+        <v>15.705843270960838</v>
+      </c>
+      <c r="S36" s="3">
+        <f t="shared" si="30"/>
+        <v>18.847011925153005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>0.4</v>
       </c>
       <c r="B37" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>10857.344210806325</v>
       </c>
       <c r="C37" s="3">
@@ -5249,13 +5849,45 @@
         <f t="shared" si="29"/>
         <v>10857.344210806325</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L37" s="3">
+        <f t="shared" si="32"/>
+        <v>21.539442200174864</v>
+      </c>
+      <c r="M37" s="3">
+        <f t="shared" si="30"/>
+        <v>28.719256266899819</v>
+      </c>
+      <c r="N37" s="3">
+        <f t="shared" si="30"/>
+        <v>35.899070333624778</v>
+      </c>
+      <c r="O37" s="3">
+        <f t="shared" si="30"/>
+        <v>43.078884400349729</v>
+      </c>
+      <c r="P37" s="3">
+        <f t="shared" si="30"/>
+        <v>10.769721100087432</v>
+      </c>
+      <c r="Q37" s="3">
+        <f t="shared" si="30"/>
+        <v>14.35962813344991</v>
+      </c>
+      <c r="R37" s="3">
+        <f t="shared" si="30"/>
+        <v>17.949535166812389</v>
+      </c>
+      <c r="S37" s="3">
+        <f t="shared" si="30"/>
+        <v>21.539442200174864</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>0.45</v>
       </c>
       <c r="B38" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>12214.512237157114</v>
       </c>
       <c r="C38" s="3">
@@ -5286,13 +5918,45 @@
         <f t="shared" si="29"/>
         <v>12214.512237157114</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L38" s="3">
+        <f t="shared" si="32"/>
+        <v>24.23187247519672</v>
+      </c>
+      <c r="M38" s="3">
+        <f t="shared" si="30"/>
+        <v>32.309163300262298</v>
+      </c>
+      <c r="N38" s="3">
+        <f t="shared" si="30"/>
+        <v>40.386454125327866</v>
+      </c>
+      <c r="O38" s="3">
+        <f t="shared" si="30"/>
+        <v>48.463744950393441</v>
+      </c>
+      <c r="P38" s="3">
+        <f t="shared" si="30"/>
+        <v>12.11593623759836</v>
+      </c>
+      <c r="Q38" s="3">
+        <f t="shared" si="30"/>
+        <v>16.154581650131149</v>
+      </c>
+      <c r="R38" s="3">
+        <f t="shared" si="30"/>
+        <v>20.193227062663933</v>
+      </c>
+      <c r="S38" s="3">
+        <f t="shared" si="30"/>
+        <v>24.23187247519672</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>0.5</v>
       </c>
       <c r="B39" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>13571.680263507906</v>
       </c>
       <c r="C39" s="3">
@@ -5323,46 +5987,77 @@
         <f t="shared" si="29"/>
         <v>13571.680263507906</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L39" s="3">
+        <f t="shared" si="32"/>
+        <v>26.92430275021858</v>
+      </c>
+      <c r="M39" s="3">
+        <f t="shared" si="30"/>
+        <v>35.899070333624778</v>
+      </c>
+      <c r="N39" s="3">
+        <f t="shared" si="30"/>
+        <v>44.873837917030968</v>
+      </c>
+      <c r="O39" s="3">
+        <f t="shared" si="30"/>
+        <v>53.848605500437159</v>
+      </c>
+      <c r="P39" s="3">
+        <f t="shared" si="30"/>
+        <v>13.46215137510929</v>
+      </c>
+      <c r="Q39" s="3">
+        <f t="shared" si="30"/>
+        <v>17.949535166812389</v>
+      </c>
+      <c r="R39" s="3">
+        <f t="shared" si="30"/>
+        <v>22.436918958515484</v>
+      </c>
+      <c r="S39" s="3">
+        <f t="shared" si="30"/>
+        <v>26.92430275021858</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="B42">
         <f>D42*(1-F42)*(1-H42)</f>
-        <v>30.004799999999999</v>
+        <v>19.345200000000002</v>
       </c>
       <c r="D42" s="3">
-        <f>16*4/2</f>
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E42" t="s">
-        <v>36</v>
-      </c>
-      <c r="F42" s="24">
-        <v>0.05</v>
+        <v>57</v>
+      </c>
+      <c r="F42" s="32">
+        <v>0.02</v>
       </c>
       <c r="G42" t="s">
-        <v>37</v>
-      </c>
-      <c r="H42" s="25">
+        <v>34</v>
+      </c>
+      <c r="H42" s="24">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="I42" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>20</v>
       </c>
@@ -5370,312 +6065,351 @@
       <c r="D43" s="8"/>
       <c r="H43" s="8"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>0.15</v>
       </c>
       <c r="B44">
         <f>_xlfn.FLOOR.MATH($B$42*1000000/32/(B31)-2)</f>
-        <v>228</v>
+        <v>146</v>
       </c>
       <c r="C44">
-        <f t="shared" ref="C44:I44" si="31">_xlfn.FLOOR.MATH($B$42*1000000/32/(C31)-2)</f>
-        <v>170</v>
+        <f t="shared" ref="C44:I44" si="33">_xlfn.FLOOR.MATH($B$42*1000000/32/(C31)-2)</f>
+        <v>109</v>
       </c>
       <c r="D44">
-        <f t="shared" si="31"/>
-        <v>136</v>
+        <f t="shared" si="33"/>
+        <v>87</v>
       </c>
       <c r="E44">
-        <f t="shared" si="31"/>
-        <v>113</v>
+        <f t="shared" si="33"/>
+        <v>72</v>
       </c>
       <c r="F44">
-        <f t="shared" si="31"/>
-        <v>458</v>
+        <f t="shared" si="33"/>
+        <v>294</v>
       </c>
       <c r="G44">
-        <f t="shared" si="31"/>
-        <v>343</v>
+        <f t="shared" si="33"/>
+        <v>220</v>
       </c>
       <c r="H44">
-        <f t="shared" si="31"/>
-        <v>274</v>
+        <f t="shared" si="33"/>
+        <v>176</v>
       </c>
       <c r="I44">
-        <f t="shared" si="31"/>
-        <v>228</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="33"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
         <v>0.2</v>
       </c>
       <c r="B45">
         <f>_xlfn.FLOOR.MATH($B$42*1000000/32/(B32)-2)</f>
-        <v>170</v>
+        <v>109</v>
       </c>
       <c r="C45">
-        <f t="shared" ref="C45:I45" si="32">_xlfn.FLOOR.MATH($B$42*1000000/32/(C32)-2)</f>
-        <v>127</v>
+        <f t="shared" ref="C45:I46" si="34">_xlfn.FLOOR.MATH($B$42*1000000/32/(C32)-2)</f>
+        <v>81</v>
       </c>
       <c r="D45">
-        <f t="shared" si="32"/>
-        <v>101</v>
+        <f t="shared" si="34"/>
+        <v>64</v>
       </c>
       <c r="E45">
-        <f t="shared" si="32"/>
-        <v>84</v>
+        <f t="shared" si="34"/>
+        <v>53</v>
       </c>
       <c r="F45">
-        <f t="shared" si="32"/>
-        <v>343</v>
+        <f t="shared" si="34"/>
+        <v>220</v>
       </c>
       <c r="G45">
-        <f t="shared" si="32"/>
-        <v>257</v>
+        <f t="shared" si="34"/>
+        <v>165</v>
       </c>
       <c r="H45">
-        <f t="shared" si="32"/>
-        <v>205</v>
+        <f t="shared" si="34"/>
+        <v>131</v>
       </c>
       <c r="I45">
-        <f t="shared" si="32"/>
-        <v>170</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="34"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
+        <v>0.22</v>
+      </c>
+      <c r="B46">
+        <f>_xlfn.FLOOR.MATH($B$42*1000000/32/(B33)-2)</f>
+        <v>99</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="34"/>
+        <v>73</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="34"/>
+        <v>58</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="34"/>
+        <v>48</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="34"/>
+        <v>200</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="34"/>
+        <v>149</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="34"/>
+        <v>119</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="34"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A47" s="11">
         <v>0.25</v>
       </c>
-      <c r="B46">
-        <f t="shared" ref="B46:I51" si="33">_xlfn.FLOOR.MATH($B$42*1000000/32/(B34)-2)</f>
-        <v>136</v>
-      </c>
-      <c r="C46">
-        <f t="shared" si="33"/>
-        <v>101</v>
-      </c>
-      <c r="D46">
-        <f t="shared" si="33"/>
-        <v>80</v>
-      </c>
-      <c r="E46">
-        <f t="shared" si="33"/>
-        <v>67</v>
-      </c>
-      <c r="F46">
-        <f t="shared" si="33"/>
-        <v>274</v>
-      </c>
-      <c r="G46">
-        <f t="shared" si="33"/>
-        <v>205</v>
-      </c>
-      <c r="H46">
-        <f t="shared" si="33"/>
-        <v>163</v>
-      </c>
-      <c r="I46">
-        <f t="shared" si="33"/>
-        <v>136</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="11">
+      <c r="B47">
+        <f t="shared" ref="B47:I52" si="35">_xlfn.FLOOR.MATH($B$42*1000000/32/(B34)-2)</f>
+        <v>87</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="35"/>
+        <v>64</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="35"/>
+        <v>51</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="35"/>
+        <v>42</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="35"/>
+        <v>176</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="35"/>
+        <v>131</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="35"/>
+        <v>104</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="35"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A48" s="11">
         <v>0.3</v>
       </c>
-      <c r="B47">
-        <f t="shared" si="33"/>
-        <v>113</v>
-      </c>
-      <c r="C47">
-        <f t="shared" si="33"/>
-        <v>84</v>
-      </c>
-      <c r="D47">
-        <f t="shared" si="33"/>
-        <v>67</v>
-      </c>
-      <c r="E47">
-        <f t="shared" si="33"/>
-        <v>55</v>
-      </c>
-      <c r="F47">
-        <f t="shared" si="33"/>
-        <v>228</v>
-      </c>
-      <c r="G47">
-        <f t="shared" si="33"/>
-        <v>170</v>
-      </c>
-      <c r="H47">
-        <f t="shared" si="33"/>
-        <v>136</v>
-      </c>
-      <c r="I47">
-        <f t="shared" si="33"/>
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="5">
-        <v>0.35</v>
-      </c>
       <c r="B48">
-        <f t="shared" si="33"/>
-        <v>96</v>
+        <f t="shared" si="35"/>
+        <v>72</v>
       </c>
       <c r="C48">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
+        <v>53</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="35"/>
+        <v>42</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="35"/>
+        <v>35</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="35"/>
+        <v>146</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="35"/>
+        <v>109</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="35"/>
+        <v>87</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="35"/>
         <v>72</v>
-      </c>
-      <c r="D48">
-        <f t="shared" si="33"/>
-        <v>57</v>
-      </c>
-      <c r="E48">
-        <f t="shared" si="33"/>
-        <v>47</v>
-      </c>
-      <c r="F48">
-        <f t="shared" si="33"/>
-        <v>195</v>
-      </c>
-      <c r="G48">
-        <f t="shared" si="33"/>
-        <v>146</v>
-      </c>
-      <c r="H48">
-        <f t="shared" si="33"/>
-        <v>116</v>
-      </c>
-      <c r="I48">
-        <f t="shared" si="33"/>
-        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="B49">
-        <f t="shared" si="33"/>
-        <v>84</v>
+        <f t="shared" si="35"/>
+        <v>61</v>
       </c>
       <c r="C49">
-        <f t="shared" si="33"/>
-        <v>62</v>
+        <f t="shared" si="35"/>
+        <v>45</v>
       </c>
       <c r="D49">
-        <f t="shared" si="33"/>
-        <v>49</v>
+        <f t="shared" si="35"/>
+        <v>36</v>
       </c>
       <c r="E49">
-        <f t="shared" si="33"/>
-        <v>41</v>
+        <f t="shared" si="35"/>
+        <v>29</v>
       </c>
       <c r="F49">
-        <f t="shared" si="33"/>
-        <v>170</v>
+        <f t="shared" si="35"/>
+        <v>125</v>
       </c>
       <c r="G49">
-        <f t="shared" si="33"/>
-        <v>127</v>
+        <f t="shared" si="35"/>
+        <v>93</v>
       </c>
       <c r="H49">
-        <f t="shared" si="33"/>
-        <v>101</v>
+        <f t="shared" si="35"/>
+        <v>74</v>
       </c>
       <c r="I49">
-        <f t="shared" si="33"/>
-        <v>84</v>
+        <f t="shared" si="35"/>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="B50">
-        <f t="shared" si="33"/>
-        <v>74</v>
+        <f t="shared" si="35"/>
+        <v>53</v>
       </c>
       <c r="C50">
-        <f t="shared" si="33"/>
-        <v>55</v>
+        <f t="shared" si="35"/>
+        <v>39</v>
       </c>
       <c r="D50">
-        <f t="shared" si="33"/>
-        <v>44</v>
+        <f t="shared" si="35"/>
+        <v>31</v>
       </c>
       <c r="E50">
-        <f t="shared" si="33"/>
-        <v>36</v>
+        <f t="shared" si="35"/>
+        <v>25</v>
       </c>
       <c r="F50">
-        <f t="shared" si="33"/>
-        <v>151</v>
+        <f t="shared" si="35"/>
+        <v>109</v>
       </c>
       <c r="G50">
-        <f t="shared" si="33"/>
-        <v>113</v>
+        <f t="shared" si="35"/>
+        <v>81</v>
       </c>
       <c r="H50">
-        <f t="shared" si="33"/>
-        <v>90</v>
+        <f t="shared" si="35"/>
+        <v>64</v>
       </c>
       <c r="I50">
-        <f t="shared" si="33"/>
-        <v>74</v>
+        <f t="shared" si="35"/>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
+        <v>0.45</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="35"/>
+        <v>47</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="35"/>
+        <v>35</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="35"/>
+        <v>27</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="35"/>
+        <v>22</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="35"/>
+        <v>96</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="35"/>
+        <v>72</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="35"/>
+        <v>57</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="35"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
         <v>0.5</v>
       </c>
-      <c r="B51">
-        <f t="shared" si="33"/>
-        <v>67</v>
-      </c>
-      <c r="C51">
-        <f t="shared" si="33"/>
-        <v>49</v>
-      </c>
-      <c r="D51">
-        <f t="shared" si="33"/>
-        <v>39</v>
-      </c>
-      <c r="E51">
-        <f t="shared" si="33"/>
-        <v>32</v>
-      </c>
-      <c r="F51">
-        <f t="shared" si="33"/>
-        <v>136</v>
-      </c>
-      <c r="G51">
-        <f t="shared" si="33"/>
-        <v>101</v>
-      </c>
-      <c r="H51">
-        <f t="shared" si="33"/>
-        <v>80</v>
-      </c>
-      <c r="I51">
-        <f t="shared" si="33"/>
-        <v>67</v>
+      <c r="B52">
+        <f t="shared" si="35"/>
+        <v>42</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="35"/>
+        <v>31</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="35"/>
+        <v>24</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="35"/>
+        <v>20</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="35"/>
+        <v>87</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="35"/>
+        <v>64</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="35"/>
+        <v>51</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="35"/>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
     <mergeCell ref="X6:AE6"/>
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="F25:I25"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="G6:N6"/>
+    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="P25:S25"/>
   </mergeCells>
   <conditionalFormatting sqref="B31:I39">
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="num" val="4000"/>
         <cfvo type="num" val="11000"/>
@@ -5686,53 +6420,66 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44:I51">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="B44:I52">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="greaterThanOrEqual">
       <formula>58</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="greaterThanOrEqual">
       <formula>43</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="lessThan">
       <formula>58</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:T20">
-    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="10" stopIfTrue="1" operator="lessThan">
       <formula>26</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="11" stopIfTrue="1" operator="lessThan">
       <formula>30</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="12" stopIfTrue="1" operator="lessThan">
       <formula>106</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="13" stopIfTrue="1" operator="lessThan">
       <formula>138</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="13" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="14" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>138</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X12:AK20">
-    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="lessThan">
       <formula>26</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>30</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="lessThan">
       <formula>106</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="5" stopIfTrue="1" operator="lessThan">
       <formula>138</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="6" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>138</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L31:S39">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="10"/>
+        <cfvo type="num" val="19"/>
+        <cfvo type="num" val="21"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5740,7 +6487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C38D8DF-F9DC-4AB2-9FDB-84FDBC18785D}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -5753,36 +6500,36 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" t="s">
-        <v>45</v>
-      </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>46</v>
+      <c r="C2" s="31" t="s">
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -5892,92 +6639,92 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B13">
         <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B15">
         <v>0.02</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E15">
         <f>PRODUCT(B12:B15)</f>
         <v>6.72</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B16">
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E16">
         <f>E15*B16</f>
         <v>33.6</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
-        <v>58</v>
+      <c r="A18" s="31" t="s">
+        <v>55</v>
       </c>
       <c r="B18">
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E18">
         <f>E16/B18</f>
         <v>2.8000000000000003</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>